<commit_message>
Added h2 to index.html
</commit_message>
<xml_diff>
--- a/playerlists/1.xlsx
+++ b/playerlists/1.xlsx
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="J1" t="n">
-        <v>127.516129633</v>
+        <v>157.545162047</v>
       </c>
     </row>
     <row r="2">
@@ -518,13 +518,13 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>126.816129633</v>
+        <v>156.845162047</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Pittsburgh_Steelers</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -559,7 +559,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>WR_Deonte_Harty</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -568,13 +568,13 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>126.721225</v>
+        <v>156.645162047</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -618,13 +618,13 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>126.648667386</v>
+        <v>156.551531256</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DST_Pittsburgh_Steelers</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -668,13 +668,13 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>126.616129633</v>
+        <v>156.260834239</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_New_York_Giants</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -704,12 +704,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -718,13 +718,13 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>126.583296487</v>
+        <v>156.245162047</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -749,17 +749,17 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>WR_Davante_Adams</t>
+          <t>WR_Hunter_Renfrow</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>126.401931936</v>
+        <v>156.179120611</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -799,12 +799,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>TE_Dan_Arnold</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Davante_Adams</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>126.383532499</v>
+        <v>156.152414929</v>
       </c>
     </row>
     <row r="9">
@@ -868,13 +868,13 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>126.348667386</v>
+        <v>155.960834239</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DST_Washington_Commanders</t>
+          <t>DST_Detroit_Lions</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -904,12 +904,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -918,13 +918,13 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>126.283296487</v>
+        <v>155.945162047</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DST_Tennessee_Titans</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -934,32 +934,32 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RB_Antonio_Gibson</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>RB_Derrick_Henry</t>
+          <t>RB_Jonathan_Taylor</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Dan_Arnold</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -968,13 +968,13 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>126.231386372</v>
+        <v>155.929415629</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DST_New_York_Giants</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Ja'Marr_Chase</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1018,13 +1018,13 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>126.216129633</v>
+        <v>155.917841067</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Washington_Commanders</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1049,17 +1049,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Hunter_Renfrow</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>126.171851363</v>
+        <v>155.879120611</v>
       </c>
     </row>
     <row r="14">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1109,22 +1109,22 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>WR_Deonte_Harty</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>126.134956244</v>
+        <v>155.86481421</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DST_Washington_Commanders</t>
+          <t>DST_New_York_Jets</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>TE_Dan_Arnold</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1168,13 +1168,13 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>126.083532499</v>
+        <v>155.851531256</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1204,27 +1204,27 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>126.029472383</v>
+        <v>155.81869531</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1249,17 +1249,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Mark_Andrews</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>WR_Calvin_Ridley</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1268,13 +1268,13 @@
         </is>
       </c>
       <c r="J17" t="n">
-        <v>126.00312566</v>
+        <v>155.716920725</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DST_Tennessee_Titans</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1304,12 +1304,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Calvin_Ridley</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1318,13 +1318,13 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>125.99232973</v>
+        <v>155.653907081</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DST_Detroit_Lions</t>
+          <t>DST_Washington_Commanders</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Dan_Arnold</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1368,13 +1368,13 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>125.916129633</v>
+        <v>155.629415629</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Washington_Commanders</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1418,13 +1418,13 @@
         </is>
       </c>
       <c r="J20" t="n">
-        <v>125.89745683</v>
+        <v>155.617841067</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Dan_Arnold</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>WR_Deonte_Harty</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1468,13 +1468,13 @@
         </is>
       </c>
       <c r="J21" t="n">
-        <v>125.853762753</v>
+        <v>155.5333956</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DST_Pittsburgh_Steelers</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1504,12 +1504,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Ja'Marr_Chase</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>WR_Deonte_Harty</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1518,13 +1518,13 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>125.821225</v>
+        <v>155.521821038</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Christian_Kirk</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1568,13 +1568,13 @@
         </is>
       </c>
       <c r="J23" t="n">
-        <v>125.783296487</v>
+        <v>155.486840481</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1599,32 +1599,32 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>125.766387604</v>
+        <v>155.460834239</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DST_Cincinnati_Bengals</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1634,17 +1634,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>RB_Antonio_Gibson</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>RB_Derrick_Henry</t>
+          <t>RB_Jonathan_Taylor</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1654,21 +1654,21 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Hunter_Renfrow</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>125.731386372</v>
+        <v>155.446284665</v>
       </c>
     </row>
     <row r="26">
@@ -1699,26 +1699,26 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Mark_Andrews</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>125.697027731</v>
+        <v>155.416920725</v>
       </c>
     </row>
     <row r="27">
@@ -1734,17 +1734,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Antonio_Gibson</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>RB_Derrick_Henry</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>RB_Jonathan_Taylor</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1754,12 +1754,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Christian_Kirk</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1768,13 +1768,13 @@
         </is>
       </c>
       <c r="J27" t="n">
-        <v>125.669145753</v>
+        <v>155.389232971</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DST_New_England_Patriots</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1799,17 +1799,17 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Hunter_Renfrow</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1818,13 +1818,13 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>125.648667386</v>
+        <v>155.379120611</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>DST_San_Francisco_49ers</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1834,17 +1834,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Antonio_Gibson</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>RB_Derrick_Henry</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>RB_Jonathan_Taylor</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1859,22 +1859,22 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>125.638505626</v>
+        <v>155.349085439</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>WR_Davante_Adams</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1918,13 +1918,13 @@
         </is>
       </c>
       <c r="J30" t="n">
-        <v>125.607027303</v>
+        <v>155.267203448</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>DST_New_Orleans_Saints</t>
+          <t>DST_New_York_Giants</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1934,12 +1934,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>RB_Antonio_Gibson</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1968,13 +1968,13 @@
         </is>
       </c>
       <c r="J31" t="n">
-        <v>125.595873267</v>
+        <v>155.251531256</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_Washington_Commanders</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1999,32 +1999,32 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Christian_Kirk</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="J32" t="n">
-        <v>125.585582607</v>
+        <v>155.186840481</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_New_York_Jets</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2049,17 +2049,17 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>WR_Ja'Marr_Chase</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2068,7 +2068,7 @@
         </is>
       </c>
       <c r="J33" t="n">
-        <v>125.574272853</v>
+        <v>155.16481421</v>
       </c>
     </row>
     <row r="34">
@@ -2099,26 +2099,26 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Hunter_Renfrow</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>WR_Deonte_Harty</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="J34" t="n">
-        <v>125.553762753</v>
+        <v>155.146284665</v>
       </c>
     </row>
     <row r="35">
@@ -2149,32 +2149,32 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>WR_Michael_Pittman_Jr.</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="J35" t="n">
-        <v>125.517255127</v>
+        <v>155.131978264</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>DST_Tennessee_Titans</t>
+          <t>DST_New_York_Jets</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2199,32 +2199,32 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>TE_Dan_Arnold</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="J36" t="n">
-        <v>125.496875249</v>
+        <v>155.11869531</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>DST_New_York_Jets</t>
+          <t>DST_Tennessee_Titans</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2249,12 +2249,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Hunter_Renfrow</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2268,13 +2268,13 @@
         </is>
       </c>
       <c r="J37" t="n">
-        <v>125.471851363</v>
+        <v>155.090412168</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2309,22 +2309,22 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Michael_Pittman_Jr.</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="J38" t="n">
-        <v>125.443203627</v>
+        <v>155.046568911</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>DST_New_York_Giants</t>
+          <t>DST_Washington_Commanders</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2368,13 +2368,13 @@
         </is>
       </c>
       <c r="J39" t="n">
-        <v>125.421225</v>
+        <v>154.967203448</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>DST_Chicago_Bears</t>
+          <t>DST_New_York_Jets</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>WR_Dante_Pettis</t>
+          <t>WR_Calvin_Ridley</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2418,13 +2418,13 @@
         </is>
       </c>
       <c r="J40" t="n">
-        <v>125.410605492</v>
+        <v>154.953907081</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DST_New_Orleans_Saints</t>
+          <t>DST_Miami_Dolphins</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2454,12 +2454,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -2468,7 +2468,7 @@
         </is>
       </c>
       <c r="J41" t="n">
-        <v>125.396875249</v>
+        <v>154.935784838</v>
       </c>
     </row>
     <row r="42">
@@ -2484,17 +2484,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RB_Antonio_Gibson</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>RB_Derrick_Henry</t>
+          <t>RB_Jonathan_Taylor</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2504,12 +2504,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Deonte_Harty</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>WR_Hunter_Renfrow</t>
+          <t>WR_Ja'Marr_Chase</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2518,13 +2518,13 @@
         </is>
       </c>
       <c r="J42" t="n">
-        <v>125.385210476</v>
+        <v>154.924210276</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>DST_New_England_Patriots</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2554,12 +2554,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>WR_Ja'Marr_Chase</t>
+          <t>WR_Dante_Pettis</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2568,13 +2568,13 @@
         </is>
       </c>
       <c r="J43" t="n">
-        <v>125.374272853</v>
+        <v>154.913256871</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>DST_New_Orleans_Saints</t>
+          <t>DST_Cincinnati_Bengals</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2584,17 +2584,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RB_Christian_McCaffrey</t>
+          <t>RB_Antonio_Gibson</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>RB_Derrick_Henry</t>
+          <t>RB_Christian_McCaffrey</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>RB_Jonathan_Taylor</t>
+          <t>RB_Derrick_Henry</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>WR_Marquez_Callaway</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2618,13 +2618,13 @@
         </is>
       </c>
       <c r="J44" t="n">
-        <v>125.338505626</v>
+        <v>154.889232971</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>DST_Miami_Dolphins</t>
+          <t>DST_Jacksonville_Jaguars</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2649,32 +2649,32 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>WR_Robert_Woods</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="J45" t="n">
-        <v>125.325627292</v>
+        <v>154.860834239</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>DST_San_Francisco_49ers</t>
+          <t>DST_New_York_Jets</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2699,17 +2699,17 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Dan_Arnold</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>WR_Jamal_Agnew</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2718,13 +2718,13 @@
         </is>
       </c>
       <c r="J46" t="n">
-        <v>125.315321649</v>
+        <v>154.8333956</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>DST_New_York_Jets</t>
+          <t>DST_Tennessee_Titans</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2749,17 +2749,17 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>WR_Calvin_Ridley</t>
+          <t>WR_Christian_Kirk</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Marvin_Jones_Jr.</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2768,13 +2768,13 @@
         </is>
       </c>
       <c r="J47" t="n">
-        <v>125.30312566</v>
+        <v>154.802512673</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>DST_Washington_Commanders</t>
+          <t>DST_Chicago_Bears</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2799,32 +2799,32 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>TE_Dan_Arnold</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>WR_Deebo_Samuel</t>
+          <t>WR_Ja'Marr_Chase</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>WR_Deonte_Harty</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Marquez_Callaway</t>
         </is>
       </c>
       <c r="J48" t="n">
-        <v>125.288627866</v>
+        <v>154.788985092</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>DST_Tennessee_Titans</t>
+          <t>DST_New_York_Jets</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2849,17 +2849,17 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>TE_Logan_Thomas</t>
+          <t>TE_Maxx_Williams</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>WR_DJ_Chark</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Jamal_Agnew</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
@@ -2868,13 +2868,13 @@
         </is>
       </c>
       <c r="J49" t="n">
-        <v>125.27580682</v>
+        <v>154.760834239</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>DST_Cincinnati_Bengals</t>
+          <t>DST_Detroit_Lions</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2899,26 +2899,26 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>TE_Maxx_Williams</t>
+          <t>TE_Logan_Thomas</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>WR_Christian_Kirk</t>
+          <t>WR_Deebo_Samuel</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>WR_Marvin_Jones_Jr.</t>
+          <t>WR_Quintez_Cephus</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>WR_Quintez_Cephus</t>
+          <t>WR_Randall_Cobb</t>
         </is>
       </c>
       <c r="J50" t="n">
-        <v>125.262010136</v>
+        <v>154.739969503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>